<commit_message>
Returning only one result
</commit_message>
<xml_diff>
--- a/findComps/Comp Tables/Competitive Market2.xlsx
+++ b/findComps/Comp Tables/Competitive Market2.xlsx
@@ -70,34 +70,34 @@
     <t>S</t>
   </si>
   <si>
-    <t>Regina Health Center</t>
-  </si>
-  <si>
-    <t>5232 BROADVIEW RD</t>
-  </si>
-  <si>
-    <t>Richfield</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>44286</t>
-  </si>
-  <si>
-    <t>3306594161</t>
+    <t>Villa At Evergreen Park,The</t>
+  </si>
+  <si>
+    <t>10124 SOUTH KEDZIE</t>
+  </si>
+  <si>
+    <t>Evergreen Park</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>60805</t>
+  </si>
+  <si>
+    <t>7089077000</t>
   </si>
   <si>
     <t>SNF</t>
   </si>
   <si>
-    <t>25.3 mi</t>
+    <t>19.7 mi</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>4</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -724,7 +724,7 @@
         <v>23</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>101</v>
+        <v>242</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>24</v>
@@ -733,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="24" t="n">
-        <v>0.9900990099009901</v>
+        <v>0.5826446280991735</v>
       </c>
       <c r="M2" s="24" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed API Key Bug
</commit_message>
<xml_diff>
--- a/findComps/Comp Tables/Competitive Market2.xlsx
+++ b/findComps/Comp Tables/Competitive Market2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
   <si>
     <t>Facility Name</t>
   </si>
@@ -70,154 +70,220 @@
     <t>S</t>
   </si>
   <si>
-    <t>Fairview Commons Nursing &amp; Rehabilitation Center</t>
-  </si>
-  <si>
-    <t>CHRISTIAN HILL ROAD</t>
-  </si>
-  <si>
-    <t>Great Barrington</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>01230</t>
-  </si>
-  <si>
-    <t>4135284560</t>
+    <t>Westpark Neurology And Rehabilitation Center</t>
+  </si>
+  <si>
+    <t>4401 W 150TH STREET</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>44135</t>
+  </si>
+  <si>
+    <t>2162527555</t>
   </si>
   <si>
     <t>SNF</t>
   </si>
   <si>
-    <t>2.9 mi</t>
+    <t>0</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>Timberlyn East Nursing And Rehabilitation</t>
-  </si>
-  <si>
-    <t>148 MAPLE AVENUE</t>
-  </si>
-  <si>
-    <t>4135283320</t>
-  </si>
-  <si>
-    <t>0.6 mi</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>Enniscourt Nursing Care</t>
+  </si>
+  <si>
+    <t>13315 DETROIT AVE</t>
+  </si>
+  <si>
+    <t>Lakewood</t>
+  </si>
+  <si>
+    <t>44107</t>
+  </si>
+  <si>
+    <t>2162263858</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Rocky River Gardens Rehab And Nursing Ctr</t>
+  </si>
+  <si>
+    <t>4102 ROCKY RIVER DR</t>
+  </si>
+  <si>
+    <t>2162513300</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Crestmont North Nursing Home</t>
+  </si>
+  <si>
+    <t>13330 DETROIT AVE</t>
+  </si>
+  <si>
+    <t>2162289550</t>
+  </si>
+  <si>
+    <t>North Park Care Center</t>
+  </si>
+  <si>
+    <t>14801 HOLLAND ROAD</t>
+  </si>
+  <si>
+    <t>Brook Park</t>
+  </si>
+  <si>
+    <t>44142</t>
+  </si>
+  <si>
+    <t>2168031995</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>Noble Horizons</t>
-  </si>
-  <si>
-    <t>17 COBBLE RD</t>
-  </si>
-  <si>
-    <t>Salisbury</t>
-  </si>
-  <si>
-    <t>CT</t>
-  </si>
-  <si>
-    <t>06068</t>
-  </si>
-  <si>
-    <t>8604359851</t>
-  </si>
-  <si>
-    <t>15.8 mi</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Kindred Nursing &amp; Rehabilitation-Laurel Lake</t>
-  </si>
-  <si>
-    <t>620 LAUREL STREET</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>01238</t>
-  </si>
-  <si>
-    <t>4132432010</t>
-  </si>
-  <si>
-    <t>14.8 mi</t>
-  </si>
-  <si>
-    <t>Timberlyn Heights Nursing And Rehabilitation</t>
-  </si>
-  <si>
-    <t>320 MAPLE AVENUE</t>
-  </si>
-  <si>
-    <t>4135282650</t>
-  </si>
-  <si>
-    <t>1 ft</t>
-  </si>
-  <si>
-    <t>Kimball Farms Nursing Care Center</t>
-  </si>
-  <si>
-    <t>40 SUNSET AVENUE</t>
-  </si>
-  <si>
-    <t>Lenox</t>
-  </si>
-  <si>
-    <t>01240</t>
-  </si>
-  <si>
-    <t>4136375011</t>
-  </si>
-  <si>
-    <t>Geer Nursing And Rehabilitation</t>
-  </si>
-  <si>
-    <t>99 SOUTH CANAAN RD</t>
-  </si>
-  <si>
-    <t>Canaan</t>
-  </si>
-  <si>
-    <t>06018</t>
-  </si>
-  <si>
-    <t>8608245137</t>
-  </si>
-  <si>
-    <t>13.7 mi</t>
-  </si>
-  <si>
-    <t>Mount Carmel Care Center</t>
-  </si>
-  <si>
-    <t>320 PITTSFIELD ROAD</t>
-  </si>
-  <si>
-    <t>4136372660</t>
-  </si>
-  <si>
-    <t>17.6 mi</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>Welsh Home The</t>
+  </si>
+  <si>
+    <t>22199 CENTER RIDGE RD</t>
+  </si>
+  <si>
+    <t>Rocky River</t>
+  </si>
+  <si>
+    <t>44116</t>
+  </si>
+  <si>
+    <t>4403310420</t>
+  </si>
+  <si>
+    <t>Rae-Ann West Park</t>
+  </si>
+  <si>
+    <t>4650 ROCKY RIVER DR</t>
+  </si>
+  <si>
+    <t>2162675445</t>
+  </si>
+  <si>
+    <t>O'Neill Healthcare Lakewood</t>
+  </si>
+  <si>
+    <t>13900 DETROIT AVE</t>
+  </si>
+  <si>
+    <t>2162287650</t>
+  </si>
+  <si>
+    <t>Normandy Manor Of Rocky River</t>
+  </si>
+  <si>
+    <t>22709 LAKE RD</t>
+  </si>
+  <si>
+    <t>4403335400</t>
+  </si>
+  <si>
+    <t>Larchwood Village Retirement Community</t>
+  </si>
+  <si>
+    <t>4110 ROCKY RIVER DRIVE</t>
+  </si>
+  <si>
+    <t>2169416100</t>
+  </si>
+  <si>
+    <t>Pleasant Lake Villa</t>
+  </si>
+  <si>
+    <t>7260 RIDGE RD</t>
+  </si>
+  <si>
+    <t>Parma</t>
+  </si>
+  <si>
+    <t>44129</t>
+  </si>
+  <si>
+    <t>4408422273</t>
+  </si>
+  <si>
+    <t>Pleasantview Care Center</t>
+  </si>
+  <si>
+    <t>7377 RIDGE RD</t>
+  </si>
+  <si>
+    <t>4408450200</t>
+  </si>
+  <si>
+    <t>O'Neill Healthcare Fairview Park</t>
+  </si>
+  <si>
+    <t>20770 LORAIN ROAD</t>
+  </si>
+  <si>
+    <t>Fairview Park</t>
+  </si>
+  <si>
+    <t>44126</t>
+  </si>
+  <si>
+    <t>4403310300</t>
+  </si>
+  <si>
+    <t>Eliza Jennings Home</t>
+  </si>
+  <si>
+    <t>10603 DETROIT AVENUE</t>
+  </si>
+  <si>
+    <t>44102</t>
+  </si>
+  <si>
+    <t>2162260282</t>
+  </si>
+  <si>
+    <t>Algart Health Care</t>
+  </si>
+  <si>
+    <t>8902 DETROIT AVE</t>
+  </si>
+  <si>
+    <t>2166311550</t>
+  </si>
+  <si>
+    <t>East Park Care Center</t>
+  </si>
+  <si>
+    <t>8 EAST PARK CIRCLE</t>
+  </si>
+  <si>
+    <t>2162677229</t>
+  </si>
+  <si>
+    <t>St Augustine Manor</t>
+  </si>
+  <si>
+    <t>7801 DETROIT AVE</t>
+  </si>
+  <si>
+    <t>2166347400</t>
   </si>
 </sst>
 </file>
@@ -844,28 +910,26 @@
         <v>23</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>180</v>
-      </c>
-      <c r="J2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="9" t="n"/>
+      <c r="K2" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="24" t="n">
+        <v>0.8251748251748252</v>
+      </c>
+      <c r="M2" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" s="24" t="s">
         <v>24</v>
-      </c>
-      <c r="K2" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="24" t="n">
-        <v>0.6611111111111111</v>
-      </c>
-      <c r="M2" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>25</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>25</v>
@@ -883,31 +947,29 @@
         <v>27</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>88</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>29</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="J3" s="25" t="n"/>
       <c r="K3" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L3" s="26" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.92</v>
       </c>
       <c r="M3" s="26" t="b">
         <v>0</v>
@@ -919,10 +981,10 @@
         <v>0</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -931,37 +993,35 @@
         <v/>
       </c>
       <c r="B4" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="8" t="n">
-        <v>110</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>38</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="J4" s="27" t="n"/>
       <c r="K4" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L4" s="24" t="n">
-        <v>0.7818181818181819</v>
+        <v>0.5785714285714286</v>
       </c>
       <c r="M4" s="24" t="b">
         <v>0</v>
@@ -970,13 +1030,13 @@
         <v>0</v>
       </c>
       <c r="O4" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -985,37 +1045,35 @@
         <v/>
       </c>
       <c r="B5" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>88</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>46</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="J5" s="25" t="n"/>
       <c r="K5" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L5" s="26" t="n">
-        <v>0.9204545454545454</v>
+        <v>0.7746478873239436</v>
       </c>
       <c r="M5" s="26" t="b">
         <v>0</v>
@@ -1027,10 +1085,10 @@
         <v>0</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1039,37 +1097,35 @@
         <v/>
       </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="8" t="n">
-        <v>71</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>50</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J6" s="27" t="n"/>
       <c r="K6" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L6" s="24" t="n">
-        <v>0.8591549295774648</v>
+        <v>0.92</v>
       </c>
       <c r="M6" s="24" t="b">
         <v>0</v>
@@ -1081,10 +1137,10 @@
         <v>0</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1093,40 +1149,38 @@
         <v/>
       </c>
       <c r="B7" s="13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>74</v>
-      </c>
-      <c r="J7" s="25" t="s">
-        <v>46</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="J7" s="25" t="n"/>
       <c r="K7" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L7" s="26" t="n">
-        <v>0.9864864864864865</v>
+        <v>0.9113924050632911</v>
       </c>
       <c r="M7" s="26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="26" t="b">
         <v>0</v>
@@ -1135,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1147,37 +1201,35 @@
         <v/>
       </c>
       <c r="B8" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="8" t="n">
-        <v>120</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>61</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="J8" s="27" t="n"/>
       <c r="K8" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L8" s="24" t="n">
-        <v>0.775</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="M8" s="24" t="b">
         <v>0</v>
@@ -1189,10 +1241,10 @@
         <v>0</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1201,40 +1253,38 @@
         <v/>
       </c>
       <c r="B9" s="13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>69</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>65</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="J9" s="25" t="n"/>
       <c r="K9" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L9" s="26" t="n">
-        <v>0.9855072463768116</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="M9" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="26" t="b">
         <v>0</v>
@@ -1243,10 +1293,10 @@
         <v>0</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1254,198 +1304,468 @@
         <f>A9+1</f>
         <v/>
       </c>
-      <c r="B10" s="6" t="n"/>
-      <c r="C10" s="6" t="n"/>
-      <c r="D10" s="6" t="n"/>
-      <c r="E10" s="6" t="n"/>
-      <c r="F10" s="9" t="n"/>
-      <c r="G10" s="9" t="n"/>
-      <c r="H10" s="9" t="n"/>
-      <c r="I10" s="8" t="n"/>
+      <c r="B10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="8" t="n">
+        <v>150</v>
+      </c>
       <c r="J10" s="27" t="n"/>
-      <c r="K10" s="10" t="n"/>
-      <c r="L10" s="24" t="n"/>
-      <c r="M10" s="24" t="n"/>
-      <c r="N10" s="24" t="n"/>
-      <c r="O10" s="24" t="n"/>
-      <c r="P10" s="24" t="n"/>
-      <c r="Q10" s="12" t="n"/>
+      <c r="K10" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="24" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="M10" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="5">
         <f>A10+1</f>
         <v/>
       </c>
-      <c r="B11" s="13" t="n"/>
-      <c r="C11" s="13" t="n"/>
-      <c r="D11" s="13" t="n"/>
-      <c r="E11" s="13" t="n"/>
-      <c r="F11" s="14" t="n"/>
-      <c r="G11" s="14" t="n"/>
-      <c r="H11" s="14" t="n"/>
-      <c r="I11" s="15" t="n"/>
+      <c r="B11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="15" t="n">
+        <v>99</v>
+      </c>
       <c r="J11" s="25" t="n"/>
-      <c r="K11" s="17" t="n"/>
-      <c r="L11" s="26" t="n"/>
-      <c r="M11" s="26" t="n"/>
-      <c r="N11" s="26" t="n"/>
-      <c r="O11" s="26" t="n"/>
-      <c r="P11" s="26" t="n"/>
-      <c r="Q11" s="19" t="n"/>
+      <c r="K11" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="26" t="n">
+        <v>0.8080808080808081</v>
+      </c>
+      <c r="M11" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="19" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="5">
         <f>A11+1</f>
         <v/>
       </c>
-      <c r="B12" s="6" t="n"/>
-      <c r="C12" s="6" t="n"/>
-      <c r="D12" s="6" t="n"/>
-      <c r="E12" s="6" t="n"/>
-      <c r="F12" s="9" t="n"/>
-      <c r="G12" s="9" t="n"/>
-      <c r="H12" s="9" t="n"/>
-      <c r="I12" s="8" t="n"/>
+      <c r="B12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="8" t="n">
+        <v>199</v>
+      </c>
       <c r="J12" s="27" t="n"/>
-      <c r="K12" s="10" t="n"/>
-      <c r="L12" s="24" t="n"/>
-      <c r="M12" s="24" t="n"/>
-      <c r="N12" s="24" t="n"/>
-      <c r="O12" s="24" t="n"/>
-      <c r="P12" s="24" t="n"/>
-      <c r="Q12" s="12" t="n"/>
+      <c r="K12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="24" t="n">
+        <v>0.8944723618090452</v>
+      </c>
+      <c r="M12" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="5">
         <f>A12+1</f>
         <v/>
       </c>
-      <c r="B13" s="13" t="n"/>
-      <c r="C13" s="13" t="n"/>
-      <c r="D13" s="13" t="n"/>
-      <c r="E13" s="13" t="n"/>
-      <c r="F13" s="14" t="n"/>
-      <c r="G13" s="14" t="n"/>
-      <c r="H13" s="14" t="n"/>
-      <c r="I13" s="15" t="n"/>
+      <c r="B13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="15" t="n">
+        <v>162</v>
+      </c>
       <c r="J13" s="25" t="n"/>
-      <c r="K13" s="17" t="n"/>
-      <c r="L13" s="26" t="n"/>
-      <c r="M13" s="26" t="n"/>
-      <c r="N13" s="26" t="n"/>
-      <c r="O13" s="26" t="n"/>
-      <c r="P13" s="26" t="n"/>
-      <c r="Q13" s="19" t="n"/>
+      <c r="K13" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="26" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="M13" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="5">
         <f>A13+1</f>
         <v/>
       </c>
-      <c r="B14" s="6" t="n"/>
-      <c r="C14" s="6" t="n"/>
-      <c r="D14" s="6" t="n"/>
-      <c r="E14" s="6" t="n"/>
-      <c r="F14" s="9" t="n"/>
-      <c r="G14" s="9" t="n"/>
-      <c r="H14" s="9" t="n"/>
-      <c r="I14" s="8" t="n"/>
+      <c r="B14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="8" t="n">
+        <v>118</v>
+      </c>
       <c r="J14" s="9" t="n"/>
-      <c r="K14" s="10" t="n"/>
-      <c r="L14" s="24" t="n"/>
-      <c r="M14" s="24" t="n"/>
-      <c r="N14" s="24" t="n"/>
-      <c r="O14" s="24" t="n"/>
-      <c r="P14" s="24" t="n"/>
-      <c r="Q14" s="12" t="n"/>
+      <c r="K14" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M14" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="5">
         <f>A14+1</f>
         <v/>
       </c>
-      <c r="B15" s="13" t="n"/>
-      <c r="C15" s="13" t="n"/>
-      <c r="D15" s="13" t="n"/>
-      <c r="E15" s="13" t="n"/>
-      <c r="F15" s="14" t="n"/>
-      <c r="G15" s="14" t="n"/>
-      <c r="H15" s="14" t="n"/>
-      <c r="I15" s="15" t="n"/>
+      <c r="B15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="15" t="n">
+        <v>126</v>
+      </c>
       <c r="J15" s="25" t="n"/>
-      <c r="K15" s="17" t="n"/>
-      <c r="L15" s="26" t="n"/>
-      <c r="M15" s="26" t="n"/>
-      <c r="N15" s="26" t="n"/>
-      <c r="O15" s="26" t="n"/>
-      <c r="P15" s="26" t="n"/>
-      <c r="Q15" s="19" t="n"/>
+      <c r="K15" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" s="26" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="M15" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P15" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="5">
         <f>A15+1</f>
         <v/>
       </c>
-      <c r="B16" s="6" t="n"/>
-      <c r="C16" s="6" t="n"/>
-      <c r="D16" s="6" t="n"/>
-      <c r="E16" s="6" t="n"/>
-      <c r="F16" s="9" t="n"/>
-      <c r="G16" s="9" t="n"/>
-      <c r="H16" s="9" t="n"/>
-      <c r="I16" s="8" t="n"/>
+      <c r="B16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="8" t="n">
+        <v>72</v>
+      </c>
       <c r="J16" s="9" t="n"/>
-      <c r="K16" s="10" t="n"/>
-      <c r="L16" s="24" t="n"/>
-      <c r="M16" s="24" t="n"/>
-      <c r="N16" s="24" t="n"/>
-      <c r="O16" s="24" t="n"/>
-      <c r="P16" s="24" t="n"/>
-      <c r="Q16" s="12" t="n"/>
+      <c r="K16" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P16" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="5">
         <f>A16+1</f>
         <v/>
       </c>
-      <c r="B17" s="13" t="n"/>
-      <c r="C17" s="13" t="n"/>
-      <c r="D17" s="13" t="n"/>
-      <c r="E17" s="13" t="n"/>
-      <c r="F17" s="14" t="n"/>
-      <c r="G17" s="14" t="n"/>
-      <c r="H17" s="14" t="n"/>
-      <c r="I17" s="15" t="n"/>
+      <c r="B17" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="15" t="n">
+        <v>63</v>
+      </c>
       <c r="J17" s="25" t="n"/>
-      <c r="K17" s="17" t="n"/>
-      <c r="L17" s="26" t="n"/>
-      <c r="M17" s="26" t="n"/>
-      <c r="N17" s="26" t="n"/>
-      <c r="O17" s="26" t="n"/>
-      <c r="P17" s="26" t="n"/>
-      <c r="Q17" s="19" t="n"/>
+      <c r="K17" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" s="26" t="n">
+        <v>0.6825396825396826</v>
+      </c>
+      <c r="M17" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P17" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="5">
         <f>A17+1</f>
         <v/>
       </c>
-      <c r="B18" s="6" t="n"/>
-      <c r="C18" s="6" t="n"/>
-      <c r="D18" s="6" t="n"/>
-      <c r="E18" s="6" t="n"/>
-      <c r="F18" s="9" t="n"/>
-      <c r="G18" s="9" t="n"/>
-      <c r="H18" s="9" t="n"/>
-      <c r="I18" s="8" t="n"/>
+      <c r="B18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="8" t="n">
+        <v>248</v>
+      </c>
       <c r="J18" s="9" t="n"/>
-      <c r="K18" s="10" t="n"/>
-      <c r="L18" s="24" t="n"/>
-      <c r="M18" s="24" t="n"/>
-      <c r="N18" s="24" t="n"/>
-      <c r="O18" s="24" t="n"/>
-      <c r="P18" s="24" t="n"/>
-      <c r="Q18" s="12" t="n"/>
+      <c r="K18" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="24" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="M18" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O18" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P18" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="5">

</xml_diff>

<commit_message>
Added in Stylized Comp Button
</commit_message>
<xml_diff>
--- a/findComps/Comp Tables/Competitive Market2.xlsx
+++ b/findComps/Comp Tables/Competitive Market2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="143">
   <si>
     <t>Facility Name</t>
   </si>
@@ -70,220 +70,382 @@
     <t>S</t>
   </si>
   <si>
-    <t>Westpark Neurology And Rehabilitation Center</t>
-  </si>
-  <si>
-    <t>4401 W 150TH STREET</t>
-  </si>
-  <si>
-    <t>Cleveland</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>44135</t>
-  </si>
-  <si>
-    <t>2162527555</t>
+    <t>Spaulding Nursing &amp; Therapy Center - North End</t>
+  </si>
+  <si>
+    <t>70 FULTON STREET</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>02109</t>
+  </si>
+  <si>
+    <t>6177269701</t>
   </si>
   <si>
     <t>SNF</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>West Revere Health Center</t>
+  </si>
+  <si>
+    <t>133 SALEM STREET</t>
+  </si>
+  <si>
+    <t>Revere</t>
+  </si>
+  <si>
+    <t>02151</t>
+  </si>
+  <si>
+    <t>7813224861</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Life Care Center Of Stoneham</t>
+  </si>
+  <si>
+    <t>25 WOODLAND ROAD</t>
+  </si>
+  <si>
+    <t>Stoneham</t>
+  </si>
+  <si>
+    <t>02180</t>
+  </si>
+  <si>
+    <t>7816622545</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Enniscourt Nursing Care</t>
-  </si>
-  <si>
-    <t>13315 DETROIT AVE</t>
-  </si>
-  <si>
-    <t>Lakewood</t>
-  </si>
-  <si>
-    <t>44107</t>
-  </si>
-  <si>
-    <t>2162263858</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Rocky River Gardens Rehab And Nursing Ctr</t>
-  </si>
-  <si>
-    <t>4102 ROCKY RIVER DR</t>
-  </si>
-  <si>
-    <t>2162513300</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>Crestmont North Nursing Home</t>
-  </si>
-  <si>
-    <t>13330 DETROIT AVE</t>
-  </si>
-  <si>
-    <t>2162289550</t>
-  </si>
-  <si>
-    <t>North Park Care Center</t>
-  </si>
-  <si>
-    <t>14801 HOLLAND ROAD</t>
-  </si>
-  <si>
-    <t>Brook Park</t>
-  </si>
-  <si>
-    <t>44142</t>
-  </si>
-  <si>
-    <t>2168031995</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Welsh Home The</t>
-  </si>
-  <si>
-    <t>22199 CENTER RIDGE RD</t>
-  </si>
-  <si>
-    <t>Rocky River</t>
-  </si>
-  <si>
-    <t>44116</t>
-  </si>
-  <si>
-    <t>4403310420</t>
-  </si>
-  <si>
-    <t>Rae-Ann West Park</t>
-  </si>
-  <si>
-    <t>4650 ROCKY RIVER DR</t>
-  </si>
-  <si>
-    <t>2162675445</t>
-  </si>
-  <si>
-    <t>O'Neill Healthcare Lakewood</t>
-  </si>
-  <si>
-    <t>13900 DETROIT AVE</t>
-  </si>
-  <si>
-    <t>2162287650</t>
-  </si>
-  <si>
-    <t>Normandy Manor Of Rocky River</t>
-  </si>
-  <si>
-    <t>22709 LAKE RD</t>
-  </si>
-  <si>
-    <t>4403335400</t>
-  </si>
-  <si>
-    <t>Larchwood Village Retirement Community</t>
-  </si>
-  <si>
-    <t>4110 ROCKY RIVER DRIVE</t>
-  </si>
-  <si>
-    <t>2169416100</t>
-  </si>
-  <si>
-    <t>Pleasant Lake Villa</t>
-  </si>
-  <si>
-    <t>7260 RIDGE RD</t>
-  </si>
-  <si>
-    <t>Parma</t>
-  </si>
-  <si>
-    <t>44129</t>
-  </si>
-  <si>
-    <t>4408422273</t>
-  </si>
-  <si>
-    <t>Pleasantview Care Center</t>
-  </si>
-  <si>
-    <t>7377 RIDGE RD</t>
-  </si>
-  <si>
-    <t>4408450200</t>
-  </si>
-  <si>
-    <t>O'Neill Healthcare Fairview Park</t>
-  </si>
-  <si>
-    <t>20770 LORAIN ROAD</t>
-  </si>
-  <si>
-    <t>Fairview Park</t>
-  </si>
-  <si>
-    <t>44126</t>
-  </si>
-  <si>
-    <t>4403310300</t>
-  </si>
-  <si>
-    <t>Eliza Jennings Home</t>
-  </si>
-  <si>
-    <t>10603 DETROIT AVENUE</t>
-  </si>
-  <si>
-    <t>44102</t>
-  </si>
-  <si>
-    <t>2162260282</t>
-  </si>
-  <si>
-    <t>Algart Health Care</t>
-  </si>
-  <si>
-    <t>8902 DETROIT AVE</t>
-  </si>
-  <si>
-    <t>2166311550</t>
-  </si>
-  <si>
-    <t>East Park Care Center</t>
-  </si>
-  <si>
-    <t>8 EAST PARK CIRCLE</t>
-  </si>
-  <si>
-    <t>2162677229</t>
-  </si>
-  <si>
-    <t>St Augustine Manor</t>
-  </si>
-  <si>
-    <t>7801 DETROIT AVE</t>
-  </si>
-  <si>
-    <t>2166347400</t>
+    <t>Chestnut Woods Rehabilitation And Healthcare Ctr</t>
+  </si>
+  <si>
+    <t>73 CHESTNUT STREET</t>
+  </si>
+  <si>
+    <t>Saugus</t>
+  </si>
+  <si>
+    <t>01906</t>
+  </si>
+  <si>
+    <t>7812338123</t>
+  </si>
+  <si>
+    <t>Dexter House Healthcare</t>
+  </si>
+  <si>
+    <t>120 MAIN STREET</t>
+  </si>
+  <si>
+    <t>Malden</t>
+  </si>
+  <si>
+    <t>02148</t>
+  </si>
+  <si>
+    <t>7813245600</t>
+  </si>
+  <si>
+    <t>Leonard Florence Center For Living</t>
+  </si>
+  <si>
+    <t>165 CAPTAIN'S ROW</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>02150</t>
+  </si>
+  <si>
+    <t>6178870001</t>
+  </si>
+  <si>
+    <t>Chelsea Jewish Nursing Home</t>
+  </si>
+  <si>
+    <t>17 LAFAYETTE AVENUE</t>
+  </si>
+  <si>
+    <t>6178846766</t>
+  </si>
+  <si>
+    <t>Courtyard Nursing Care Center</t>
+  </si>
+  <si>
+    <t>200 GOVERNORS AVENUE</t>
+  </si>
+  <si>
+    <t>Medford</t>
+  </si>
+  <si>
+    <t>02155</t>
+  </si>
+  <si>
+    <t>7813915400</t>
+  </si>
+  <si>
+    <t>Elmhurst Healthcare (The)</t>
+  </si>
+  <si>
+    <t>743 MAIN STREET</t>
+  </si>
+  <si>
+    <t>Melrose</t>
+  </si>
+  <si>
+    <t>02176</t>
+  </si>
+  <si>
+    <t>7816627500</t>
+  </si>
+  <si>
+    <t>Armenian Nursing &amp; Rehabilitation Center</t>
+  </si>
+  <si>
+    <t>431 POND STREET</t>
+  </si>
+  <si>
+    <t>02130</t>
+  </si>
+  <si>
+    <t>6175222600</t>
+  </si>
+  <si>
+    <t>Care One At Brookline</t>
+  </si>
+  <si>
+    <t>99 PARK STREET</t>
+  </si>
+  <si>
+    <t>Brookline</t>
+  </si>
+  <si>
+    <t>02146</t>
+  </si>
+  <si>
+    <t>6177311050</t>
+  </si>
+  <si>
+    <t>Rehabilitation &amp; Nursing Center At Everett (The)</t>
+  </si>
+  <si>
+    <t>289 ELM STREET</t>
+  </si>
+  <si>
+    <t>Everett</t>
+  </si>
+  <si>
+    <t>02149</t>
+  </si>
+  <si>
+    <t>6173876560</t>
+  </si>
+  <si>
+    <t>Marian Manor</t>
+  </si>
+  <si>
+    <t>130 DORCHESTER AVENUE</t>
+  </si>
+  <si>
+    <t>02127</t>
+  </si>
+  <si>
+    <t>6172683333</t>
+  </si>
+  <si>
+    <t>Sherrill House</t>
+  </si>
+  <si>
+    <t>135 SOUTH HUNTINGTON AVENUE</t>
+  </si>
+  <si>
+    <t>6177312400</t>
+  </si>
+  <si>
+    <t>Kindred Nursing &amp; Rehabilitation-Harborlights</t>
+  </si>
+  <si>
+    <t>804 EAST 7TH STREET</t>
+  </si>
+  <si>
+    <t>6172688968</t>
+  </si>
+  <si>
+    <t>Melrose Healthcare</t>
+  </si>
+  <si>
+    <t>40 MARTIN STREET</t>
+  </si>
+  <si>
+    <t>7816657050</t>
+  </si>
+  <si>
+    <t>Jeanne Jugan Residence</t>
+  </si>
+  <si>
+    <t>186 HIGHLAND AVENUE</t>
+  </si>
+  <si>
+    <t>Somerville</t>
+  </si>
+  <si>
+    <t>02143</t>
+  </si>
+  <si>
+    <t>6177764420</t>
+  </si>
+  <si>
+    <t>Don Orione Nursing Home</t>
+  </si>
+  <si>
+    <t>111 ORIENT AVENUE</t>
+  </si>
+  <si>
+    <t>02128</t>
+  </si>
+  <si>
+    <t>6175692100</t>
+  </si>
+  <si>
+    <t>Medford Rehabilitation And Nursing Center</t>
+  </si>
+  <si>
+    <t>300 WINTHROP STREET</t>
+  </si>
+  <si>
+    <t>7813964400</t>
+  </si>
+  <si>
+    <t>Lighthouse Nursing Care Center</t>
+  </si>
+  <si>
+    <t>204 PROCTOR AVENUE</t>
+  </si>
+  <si>
+    <t>7812863100</t>
+  </si>
+  <si>
+    <t>Saugus Center</t>
+  </si>
+  <si>
+    <t>266 LINCOLN AVENUE</t>
+  </si>
+  <si>
+    <t>7812336830</t>
+  </si>
+  <si>
+    <t>Laurel Ridge Rehab And Skilled Care Center</t>
+  </si>
+  <si>
+    <t>174 FOREST HILLS STREET</t>
+  </si>
+  <si>
+    <t>6175221550</t>
+  </si>
+  <si>
+    <t>Benjamin Healthcare Center</t>
+  </si>
+  <si>
+    <t>120 FISHER AVENUE</t>
+  </si>
+  <si>
+    <t>02120</t>
+  </si>
+  <si>
+    <t>6177381500</t>
+  </si>
+  <si>
+    <t>Glen Ridge Nursing Care Center</t>
+  </si>
+  <si>
+    <t>120 MURRAY STREET</t>
+  </si>
+  <si>
+    <t>7813910800</t>
+  </si>
+  <si>
+    <t>Eastpointe Rehab Center</t>
+  </si>
+  <si>
+    <t>255 CENTRAL AVENUE</t>
+  </si>
+  <si>
+    <t>6178845700</t>
+  </si>
+  <si>
+    <t>Wakefield Center</t>
+  </si>
+  <si>
+    <t>ONE BATHOL STREET</t>
+  </si>
+  <si>
+    <t>Wakefield</t>
+  </si>
+  <si>
+    <t>01880</t>
+  </si>
+  <si>
+    <t>7812457600</t>
+  </si>
+  <si>
+    <t>Soldiers Home In Massachusetts</t>
+  </si>
+  <si>
+    <t>91 CREST AVENUE</t>
+  </si>
+  <si>
+    <t>6178845660</t>
+  </si>
+  <si>
+    <t>Chelsea Skilled Nursing And Rehabilitation</t>
+  </si>
+  <si>
+    <t>932 BROADWAY</t>
+  </si>
+  <si>
+    <t>6178892250</t>
+  </si>
+  <si>
+    <t>Greenwood Nursing &amp; Rehabilitation Center</t>
+  </si>
+  <si>
+    <t>90 GREENWOOD STREET</t>
+  </si>
+  <si>
+    <t>7812460211</t>
+  </si>
+  <si>
+    <t>Bear Hill Nursing Center At Wakefield</t>
+  </si>
+  <si>
+    <t>ENTER 11 NORTH STREET</t>
+  </si>
+  <si>
+    <t>7814388515</t>
   </si>
 </sst>
 </file>
@@ -910,14 +1072,14 @@
         <v>23</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J2" s="9" t="n"/>
       <c r="K2" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L2" s="24" t="n">
-        <v>0.8251748251748252</v>
+        <v>0.8642857142857143</v>
       </c>
       <c r="M2" s="24" t="b">
         <v>0</v>
@@ -962,14 +1124,14 @@
         <v>23</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="J3" s="25" t="n"/>
       <c r="K3" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L3" s="26" t="n">
-        <v>0.92</v>
+        <v>0.6214285714285714</v>
       </c>
       <c r="M3" s="26" t="b">
         <v>0</v>
@@ -999,29 +1161,29 @@
         <v>34</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="8" t="n">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="J4" s="27" t="n"/>
       <c r="K4" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L4" s="24" t="n">
-        <v>0.5785714285714286</v>
+        <v>0.9042553191489362</v>
       </c>
       <c r="M4" s="24" t="b">
         <v>0</v>
@@ -1030,13 +1192,13 @@
         <v>0</v>
       </c>
       <c r="O4" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1045,35 +1207,35 @@
         <v/>
       </c>
       <c r="B5" s="13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="J5" s="25" t="n"/>
       <c r="K5" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L5" s="26" t="n">
-        <v>0.7746478873239436</v>
+        <v>0.9318181818181818</v>
       </c>
       <c r="M5" s="26" t="b">
         <v>0</v>
@@ -1088,7 +1250,7 @@
         <v>24</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1097,35 +1259,35 @@
         <v/>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="8" t="n">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="J6" s="27" t="n"/>
       <c r="K6" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L6" s="24" t="n">
-        <v>0.92</v>
+        <v>0.6692307692307692</v>
       </c>
       <c r="M6" s="24" t="b">
         <v>0</v>
@@ -1137,10 +1299,10 @@
         <v>0</v>
       </c>
       <c r="P6" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="Q6" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1149,35 +1311,35 @@
         <v/>
       </c>
       <c r="B7" s="13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="J7" s="25" t="n"/>
       <c r="K7" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L7" s="26" t="n">
-        <v>0.9113924050632911</v>
+        <v>0.93</v>
       </c>
       <c r="M7" s="26" t="b">
         <v>0</v>
@@ -1189,10 +1351,10 @@
         <v>0</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1201,35 +1363,35 @@
         <v/>
       </c>
       <c r="B8" s="6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="8" t="n">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="J8" s="27" t="n"/>
       <c r="K8" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L8" s="24" t="n">
-        <v>0.6428571428571429</v>
+        <v>0.8943089430894309</v>
       </c>
       <c r="M8" s="24" t="b">
         <v>0</v>
@@ -1241,10 +1403,10 @@
         <v>0</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1253,38 +1415,38 @@
         <v/>
       </c>
       <c r="B9" s="13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>135</v>
+        <v>224</v>
       </c>
       <c r="J9" s="25" t="n"/>
       <c r="K9" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L9" s="26" t="n">
-        <v>0.7333333333333333</v>
+        <v>0.9732142857142857</v>
       </c>
       <c r="M9" s="26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="26" t="b">
         <v>0</v>
@@ -1293,10 +1455,10 @@
         <v>0</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1305,35 +1467,35 @@
         <v/>
       </c>
       <c r="B10" s="6" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="8" t="n">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="J10" s="27" t="n"/>
       <c r="K10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L10" s="24" t="n">
-        <v>0.88</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="M10" s="24" t="b">
         <v>0</v>
@@ -1345,10 +1507,10 @@
         <v>0</v>
       </c>
       <c r="P10" s="24" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1357,10 +1519,10 @@
         <v/>
       </c>
       <c r="B11" s="13" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>19</v>
@@ -1369,23 +1531,23 @@
         <v>20</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="15" t="n">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="J11" s="25" t="n"/>
       <c r="K11" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L11" s="26" t="n">
-        <v>0.8080808080808081</v>
+        <v>0.927710843373494</v>
       </c>
       <c r="M11" s="26" t="b">
         <v>0</v>
@@ -1397,10 +1559,10 @@
         <v>0</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1409,35 +1571,35 @@
         <v/>
       </c>
       <c r="B12" s="6" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="8" t="n">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="J12" s="27" t="n"/>
       <c r="K12" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L12" s="24" t="n">
-        <v>0.8944723618090452</v>
+        <v>0.9416666666666667</v>
       </c>
       <c r="M12" s="24" t="b">
         <v>0</v>
@@ -1449,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1461,35 +1623,35 @@
         <v/>
       </c>
       <c r="B13" s="13" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="15" t="n">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="J13" s="25" t="n"/>
       <c r="K13" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L13" s="26" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7158469945355191</v>
       </c>
       <c r="M13" s="26" t="b">
         <v>0</v>
@@ -1501,10 +1663,10 @@
         <v>0</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="Q13" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1513,35 +1675,35 @@
         <v/>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I14" s="8" t="n">
-        <v>118</v>
+        <v>344</v>
       </c>
       <c r="J14" s="9" t="n"/>
       <c r="K14" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L14" s="24" t="n">
-        <v>0.5</v>
+        <v>0.5116279069767442</v>
       </c>
       <c r="M14" s="24" t="b">
         <v>0</v>
@@ -1556,7 +1718,7 @@
         <v>24</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1565,10 +1727,10 @@
         <v/>
       </c>
       <c r="B15" s="13" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>19</v>
@@ -1577,23 +1739,23 @@
         <v>20</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="15" t="n">
-        <v>126</v>
+        <v>196</v>
       </c>
       <c r="J15" s="25" t="n"/>
       <c r="K15" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L15" s="26" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9030612244897959</v>
       </c>
       <c r="M15" s="26" t="b">
         <v>0</v>
@@ -1605,10 +1767,10 @@
         <v>0</v>
       </c>
       <c r="P15" s="26" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1617,10 +1779,10 @@
         <v/>
       </c>
       <c r="B16" s="6" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>19</v>
@@ -1629,23 +1791,23 @@
         <v>20</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I16" s="8" t="n">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="J16" s="9" t="n"/>
       <c r="K16" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L16" s="24" t="n">
-        <v>1</v>
+        <v>0.9213483146067416</v>
       </c>
       <c r="M16" s="24" t="b">
         <v>0</v>
@@ -1657,10 +1819,10 @@
         <v>0</v>
       </c>
       <c r="P16" s="24" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1669,38 +1831,38 @@
         <v/>
       </c>
       <c r="B17" s="13" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="15" t="n">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="J17" s="25" t="n"/>
       <c r="K17" s="17" t="b">
         <v>0</v>
       </c>
       <c r="L17" s="26" t="n">
-        <v>0.6825396825396826</v>
+        <v>0.8490566037735849</v>
       </c>
       <c r="M17" s="26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="26" t="b">
         <v>0</v>
@@ -1709,10 +1871,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q17" s="19" t="s">
         <v>24</v>
-      </c>
-      <c r="Q17" s="19" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1721,35 +1883,35 @@
         <v/>
       </c>
       <c r="B18" s="6" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I18" s="8" t="n">
-        <v>248</v>
+        <v>26</v>
       </c>
       <c r="J18" s="9" t="n"/>
       <c r="K18" s="10" t="b">
         <v>0</v>
       </c>
       <c r="L18" s="24" t="n">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="M18" s="24" t="b">
         <v>0</v>
@@ -1761,10 +1923,10 @@
         <v>0</v>
       </c>
       <c r="P18" s="24" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1772,286 +1934,676 @@
         <f>A18+1</f>
         <v/>
       </c>
-      <c r="B19" s="13" t="n"/>
-      <c r="C19" s="13" t="n"/>
-      <c r="D19" s="13" t="n"/>
-      <c r="E19" s="13" t="n"/>
-      <c r="F19" s="14" t="n"/>
-      <c r="G19" s="14" t="n"/>
-      <c r="H19" s="14" t="n"/>
-      <c r="I19" s="15" t="n"/>
+      <c r="B19" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="15" t="n">
+        <v>190</v>
+      </c>
       <c r="J19" s="25" t="n"/>
-      <c r="K19" s="17" t="n"/>
-      <c r="L19" s="26" t="n"/>
-      <c r="M19" s="26" t="n"/>
-      <c r="N19" s="26" t="n"/>
-      <c r="O19" s="26" t="n"/>
-      <c r="P19" s="26" t="n"/>
-      <c r="Q19" s="19" t="n"/>
+      <c r="K19" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" s="26" t="n">
+        <v>0.6157894736842106</v>
+      </c>
+      <c r="M19" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P19" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="19" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="20" spans="1:17">
       <c r="A20" s="5">
         <f>A19+1</f>
         <v/>
       </c>
-      <c r="B20" s="6" t="n"/>
-      <c r="C20" s="6" t="n"/>
-      <c r="D20" s="6" t="n"/>
-      <c r="E20" s="6" t="n"/>
-      <c r="F20" s="9" t="n"/>
-      <c r="G20" s="9" t="n"/>
-      <c r="H20" s="9" t="n"/>
-      <c r="I20" s="8" t="n"/>
+      <c r="B20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="8" t="n">
+        <v>142</v>
+      </c>
       <c r="J20" s="9" t="n"/>
-      <c r="K20" s="10" t="n"/>
-      <c r="L20" s="24" t="n"/>
-      <c r="M20" s="24" t="n"/>
-      <c r="N20" s="24" t="n"/>
-      <c r="O20" s="24" t="n"/>
-      <c r="P20" s="24" t="n"/>
-      <c r="Q20" s="12" t="n"/>
+      <c r="K20" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" s="24" t="n">
+        <v>0.9014084507042254</v>
+      </c>
+      <c r="M20" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="5">
         <f>A20+1</f>
         <v/>
       </c>
-      <c r="B21" s="13" t="n"/>
-      <c r="C21" s="13" t="n"/>
-      <c r="D21" s="13" t="n"/>
-      <c r="E21" s="13" t="n"/>
-      <c r="F21" s="14" t="n"/>
-      <c r="G21" s="14" t="n"/>
-      <c r="H21" s="14" t="n"/>
-      <c r="I21" s="15" t="n"/>
+      <c r="B21" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="15" t="n">
+        <v>123</v>
+      </c>
       <c r="J21" s="25" t="n"/>
-      <c r="K21" s="17" t="n"/>
-      <c r="L21" s="26" t="n"/>
-      <c r="M21" s="26" t="n"/>
-      <c r="N21" s="26" t="n"/>
-      <c r="O21" s="26" t="n"/>
-      <c r="P21" s="26" t="n"/>
-      <c r="Q21" s="19" t="n"/>
+      <c r="K21" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="26" t="n">
+        <v>0.9105691056910569</v>
+      </c>
+      <c r="M21" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P21" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="5">
         <f>A21+1</f>
         <v/>
       </c>
-      <c r="B22" s="6" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="6" t="n"/>
-      <c r="E22" s="6" t="n"/>
-      <c r="F22" s="9" t="n"/>
-      <c r="G22" s="9" t="n"/>
-      <c r="H22" s="9" t="n"/>
-      <c r="I22" s="8" t="n"/>
+      <c r="B22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="8" t="n">
+        <v>80</v>
+      </c>
       <c r="J22" s="9" t="n"/>
-      <c r="K22" s="10" t="n"/>
-      <c r="L22" s="24" t="n"/>
-      <c r="M22" s="24" t="n"/>
-      <c r="N22" s="24" t="n"/>
-      <c r="O22" s="24" t="n"/>
-      <c r="P22" s="24" t="n"/>
-      <c r="Q22" s="12" t="n"/>
+      <c r="K22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" s="24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M22" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P22" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q22" s="12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="5">
         <f>A22+1</f>
         <v/>
       </c>
-      <c r="B23" s="13" t="n"/>
-      <c r="C23" s="13" t="n"/>
-      <c r="D23" s="13" t="n"/>
-      <c r="E23" s="13" t="n"/>
-      <c r="F23" s="14" t="n"/>
-      <c r="G23" s="14" t="n"/>
-      <c r="H23" s="14" t="n"/>
-      <c r="I23" s="15" t="n"/>
+      <c r="B23" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="15" t="n">
+        <v>120</v>
+      </c>
       <c r="J23" s="25" t="n"/>
-      <c r="K23" s="17" t="n"/>
-      <c r="L23" s="26" t="n"/>
-      <c r="M23" s="26" t="n"/>
-      <c r="N23" s="26" t="n"/>
-      <c r="O23" s="26" t="n"/>
-      <c r="P23" s="26" t="n"/>
-      <c r="Q23" s="19" t="n"/>
+      <c r="K23" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" s="26" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M23" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="P23" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q23" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="5">
         <f>A23+1</f>
         <v/>
       </c>
-      <c r="B24" s="6" t="n"/>
-      <c r="C24" s="6" t="n"/>
-      <c r="D24" s="6" t="n"/>
-      <c r="E24" s="6" t="n"/>
-      <c r="F24" s="9" t="n"/>
-      <c r="G24" s="9" t="n"/>
-      <c r="H24" s="9" t="n"/>
-      <c r="I24" s="8" t="n"/>
+      <c r="B24" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="8" t="n">
+        <v>205</v>
+      </c>
       <c r="J24" s="9" t="n"/>
-      <c r="K24" s="10" t="n"/>
-      <c r="L24" s="24" t="n"/>
-      <c r="M24" s="24" t="n"/>
-      <c r="N24" s="24" t="n"/>
-      <c r="O24" s="24" t="n"/>
-      <c r="P24" s="24" t="n"/>
-      <c r="Q24" s="12" t="n"/>
+      <c r="K24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" s="24" t="n">
+        <v>0.7658536585365854</v>
+      </c>
+      <c r="M24" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P24" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q24" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="5">
         <f>A24+1</f>
         <v/>
       </c>
-      <c r="B25" s="13" t="n"/>
-      <c r="C25" s="13" t="n"/>
-      <c r="D25" s="13" t="n"/>
-      <c r="E25" s="13" t="n"/>
-      <c r="F25" s="14" t="n"/>
-      <c r="G25" s="14" t="n"/>
-      <c r="H25" s="14" t="n"/>
-      <c r="I25" s="15" t="n"/>
+      <c r="B25" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="15" t="n">
+        <v>164</v>
+      </c>
       <c r="J25" s="25" t="n"/>
-      <c r="K25" s="17" t="n"/>
-      <c r="L25" s="26" t="n"/>
-      <c r="M25" s="26" t="n"/>
-      <c r="N25" s="26" t="n"/>
-      <c r="O25" s="26" t="n"/>
-      <c r="P25" s="26" t="n"/>
-      <c r="Q25" s="19" t="n"/>
+      <c r="K25" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" s="26" t="n">
+        <v>0.9024390243902439</v>
+      </c>
+      <c r="M25" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O25" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P25" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="5">
         <f>A25+1</f>
         <v/>
       </c>
-      <c r="B26" s="6" t="n"/>
-      <c r="C26" s="6" t="n"/>
-      <c r="D26" s="6" t="n"/>
-      <c r="E26" s="6" t="n"/>
-      <c r="F26" s="9" t="n"/>
-      <c r="G26" s="9" t="n"/>
-      <c r="H26" s="9" t="n"/>
-      <c r="I26" s="8" t="n"/>
+      <c r="B26" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="8" t="n">
+        <v>195</v>
+      </c>
       <c r="J26" s="9" t="n"/>
-      <c r="K26" s="10" t="n"/>
-      <c r="L26" s="24" t="n"/>
-      <c r="M26" s="24" t="n"/>
-      <c r="N26" s="24" t="n"/>
-      <c r="O26" s="24" t="n"/>
-      <c r="P26" s="24" t="n"/>
-      <c r="Q26" s="12" t="n"/>
+      <c r="K26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" s="24" t="n">
+        <v>0.9435897435897436</v>
+      </c>
+      <c r="M26" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q26" s="12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="5">
         <f>A26+1</f>
         <v/>
       </c>
-      <c r="B27" s="13" t="n"/>
-      <c r="C27" s="13" t="n"/>
-      <c r="D27" s="13" t="n"/>
-      <c r="E27" s="13" t="n"/>
-      <c r="F27" s="14" t="n"/>
-      <c r="G27" s="14" t="n"/>
-      <c r="H27" s="14" t="n"/>
-      <c r="I27" s="15" t="n"/>
+      <c r="B27" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="15" t="n">
+        <v>149</v>
+      </c>
       <c r="J27" s="25" t="n"/>
-      <c r="K27" s="17" t="n"/>
-      <c r="L27" s="26" t="n"/>
-      <c r="M27" s="26" t="n"/>
-      <c r="N27" s="26" t="n"/>
-      <c r="O27" s="26" t="n"/>
-      <c r="P27" s="26" t="n"/>
-      <c r="Q27" s="19" t="n"/>
+      <c r="K27" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" s="26" t="n">
+        <v>0.8389261744966443</v>
+      </c>
+      <c r="M27" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O27" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P27" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q27" s="19" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="5">
         <f>A27+1</f>
         <v/>
       </c>
-      <c r="B28" s="6" t="n"/>
-      <c r="C28" s="6" t="n"/>
-      <c r="D28" s="6" t="n"/>
-      <c r="E28" s="6" t="n"/>
-      <c r="F28" s="9" t="n"/>
-      <c r="G28" s="9" t="n"/>
-      <c r="H28" s="9" t="n"/>
-      <c r="I28" s="8" t="n"/>
+      <c r="B28" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="8" t="n">
+        <v>88</v>
+      </c>
       <c r="J28" s="9" t="n"/>
-      <c r="K28" s="10" t="n"/>
-      <c r="L28" s="24" t="n"/>
-      <c r="M28" s="24" t="n"/>
-      <c r="N28" s="24" t="n"/>
-      <c r="O28" s="24" t="n"/>
-      <c r="P28" s="24" t="n"/>
-      <c r="Q28" s="12" t="n"/>
+      <c r="K28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" s="24" t="n">
+        <v>0.6931818181818182</v>
+      </c>
+      <c r="M28" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O28" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q28" s="12" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="5">
         <f>A28+1</f>
         <v/>
       </c>
-      <c r="B29" s="13" t="n"/>
-      <c r="C29" s="13" t="n"/>
-      <c r="D29" s="13" t="n"/>
-      <c r="E29" s="13" t="n"/>
-      <c r="F29" s="14" t="n"/>
-      <c r="G29" s="14" t="n"/>
-      <c r="H29" s="14" t="n"/>
-      <c r="I29" s="15" t="n"/>
+      <c r="B29" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="15" t="n">
+        <v>82</v>
+      </c>
       <c r="J29" s="25" t="n"/>
-      <c r="K29" s="17" t="n"/>
-      <c r="L29" s="26" t="n"/>
-      <c r="M29" s="26" t="n"/>
-      <c r="N29" s="26" t="n"/>
-      <c r="O29" s="26" t="n"/>
-      <c r="P29" s="26" t="n"/>
-      <c r="Q29" s="19" t="n"/>
+      <c r="K29" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" s="26" t="n">
+        <v>0.7682926829268293</v>
+      </c>
+      <c r="M29" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N29" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P29" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q29" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="5">
         <f>A29+1</f>
         <v/>
       </c>
-      <c r="B30" s="6" t="n"/>
-      <c r="C30" s="6" t="n"/>
-      <c r="D30" s="6" t="n"/>
-      <c r="E30" s="6" t="n"/>
-      <c r="F30" s="9" t="n"/>
-      <c r="G30" s="9" t="n"/>
-      <c r="H30" s="9" t="n"/>
-      <c r="I30" s="8" t="n"/>
+      <c r="B30" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="8" t="n">
+        <v>36</v>
+      </c>
       <c r="J30" s="9" t="n"/>
-      <c r="K30" s="10" t="n"/>
-      <c r="L30" s="24" t="n"/>
-      <c r="M30" s="24" t="n"/>
-      <c r="N30" s="24" t="n"/>
-      <c r="O30" s="24" t="n"/>
-      <c r="P30" s="24" t="n"/>
-      <c r="Q30" s="12" t="n"/>
+      <c r="K30" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" s="24" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="M30" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="N30" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O30" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P30" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q30" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" s="5">
         <f>A30+1</f>
         <v/>
       </c>
-      <c r="B31" s="13" t="n"/>
-      <c r="C31" s="13" t="n"/>
-      <c r="D31" s="13" t="n"/>
-      <c r="E31" s="13" t="n"/>
-      <c r="F31" s="14" t="n"/>
-      <c r="G31" s="14" t="n"/>
-      <c r="H31" s="14" t="n"/>
-      <c r="I31" s="15" t="n"/>
+      <c r="B31" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="15" t="n">
+        <v>169</v>
+      </c>
       <c r="J31" s="25" t="n"/>
-      <c r="K31" s="17" t="n"/>
-      <c r="L31" s="26" t="n"/>
-      <c r="M31" s="26" t="n"/>
-      <c r="N31" s="26" t="n"/>
-      <c r="O31" s="26" t="n"/>
-      <c r="P31" s="26" t="n"/>
-      <c r="Q31" s="19" t="n"/>
+      <c r="K31" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" s="26" t="n">
+        <v>0.9585798816568047</v>
+      </c>
+      <c r="M31" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N31" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O31" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q31" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" s="5">

</xml_diff>

<commit_message>
Refactored Processing Code; Need to Handle Invalid Addresses; Create Form for Dynamic Address Entry
</commit_message>
<xml_diff>
--- a/findComps/Comp Tables/Competitive Market2.xlsx
+++ b/findComps/Comp Tables/Competitive Market2.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <bookViews>
-    <workbookView activeTab="0"/>
-  </bookViews>
-  <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Competitive Market" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Competitive Market" sheetId="1" r:id="rId1"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Facility Name</t>
   </si>
@@ -70,48 +70,57 @@
     <t>S</t>
   </si>
   <si>
-    <t>Westpark Neurology And Rehabilitation Center</t>
-  </si>
-  <si>
-    <t>4401 W 150TH STREET</t>
-  </si>
-  <si>
-    <t>Cleveland</t>
+    <t>O'Neill Healthcare Lakewood</t>
+  </si>
+  <si>
+    <t>13900 DETROIT AVE</t>
+  </si>
+  <si>
+    <t>Lakewood</t>
   </si>
   <si>
     <t>OH</t>
   </si>
   <si>
-    <t>44135</t>
-  </si>
-  <si>
-    <t>2162527555</t>
+    <t>44107</t>
+  </si>
+  <si>
+    <t>2162287650</t>
   </si>
   <si>
     <t>SNF</t>
   </si>
   <si>
-    <t>2.8 mi</t>
+    <t>2.4 mi</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Crestmont North Nursing Home</t>
+  </si>
+  <si>
+    <t>13330 DETROIT AVE</t>
+  </si>
+  <si>
+    <t>2162289550</t>
+  </si>
+  <si>
+    <t>2.7 mi</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Enniscourt Nursing Care</t>
   </si>
   <si>
     <t>13315 DETROIT AVE</t>
   </si>
   <si>
-    <t>Lakewood</t>
-  </si>
-  <si>
-    <t>44107</t>
-  </si>
-  <si>
     <t>2162263858</t>
   </si>
   <si>
@@ -122,69 +131,6 @@
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>Crestmont North Nursing Home</t>
-  </si>
-  <si>
-    <t>13330 DETROIT AVE</t>
-  </si>
-  <si>
-    <t>2162289550</t>
-  </si>
-  <si>
-    <t>2.7 mi</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Rae-Ann West Park</t>
-  </si>
-  <si>
-    <t>4650 ROCKY RIVER DR</t>
-  </si>
-  <si>
-    <t>2162675445</t>
-  </si>
-  <si>
-    <t>3.0 mi</t>
-  </si>
-  <si>
-    <t>O'Neill Healthcare Lakewood</t>
-  </si>
-  <si>
-    <t>13900 DETROIT AVE</t>
-  </si>
-  <si>
-    <t>2162287650</t>
-  </si>
-  <si>
-    <t>2.4 mi</t>
-  </si>
-  <si>
-    <t>Larchwood Village Retirement Community</t>
-  </si>
-  <si>
-    <t>4110 ROCKY RIVER DRIVE</t>
-  </si>
-  <si>
-    <t>2169416100</t>
-  </si>
-  <si>
-    <t>2.2 mi</t>
-  </si>
-  <si>
-    <t>Rocky River Gardens Rehab And Nursing Ctr</t>
-  </si>
-  <si>
-    <t>4102 ROCKY RIVER DR</t>
-  </si>
-  <si>
-    <t>2162513300</t>
-  </si>
-  <si>
-    <t>1.9 mi</t>
   </si>
 </sst>
 </file>
@@ -235,6 +181,7 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <b val="1"/>
+      <color rgb="00000000"/>
       <sz val="10"/>
     </font>
     <font>
@@ -294,116 +241,97 @@
   </borders>
   <cellStyleXfs count="5">
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="164"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+  <cellXfs count="24">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="2">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="3">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="1" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="3" xfId="3">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="165" xfId="4">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="1" xfId="4">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="3">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="1" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="166" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="3" xfId="3">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="165" xfId="4">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="4">
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="1" xfId="4">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="166" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="1" xfId="2">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="165" xfId="2">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="4">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="6" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="4">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="6" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="3" fontId="4" numFmtId="166" xfId="2">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle name="Normal 5" xfId="1"/>
+    <cellStyle name="Normal 3 3 3 2 2" xfId="1"/>
     <cellStyle name="BP Chart Head" xfId="2"/>
-    <cellStyle name="Normal 3 3 3 2 2" xfId="3"/>
+    <cellStyle name="Normal 5" xfId="3"/>
     <cellStyle name="Percent 4" xfId="4"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -715,7 +643,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="2" min="2" width="40.21875"/>
     <col customWidth="1" max="3" min="3" width="22.5546875"/>
@@ -811,7 +739,7 @@
         <v>23</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>24</v>
@@ -819,19 +747,19 @@
       <c r="K2" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="L2" s="24" t="n">
-        <v>0.8601398601398601</v>
-      </c>
-      <c r="M2" s="24" t="b">
+      <c r="L2" s="11" t="n">
+        <v>0.7333333333333333</v>
+      </c>
+      <c r="M2" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="N2" s="24" t="b">
+      <c r="O2" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="O2" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="11" t="s">
         <v>25</v>
       </c>
       <c r="Q2" s="12" t="s">
@@ -850,46 +778,46 @@
         <v>28</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>50</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="K3" s="17" t="b">
         <v>0</v>
       </c>
-      <c r="L3" s="26" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="M3" s="26" t="b">
+      <c r="L3" s="18" t="n">
+        <v>0.7746478873239436</v>
+      </c>
+      <c r="M3" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="N3" s="26" t="b">
+      <c r="N3" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="O3" s="26" t="b">
+      <c r="O3" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="P3" s="26" t="s">
-        <v>33</v>
+      <c r="P3" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -898,52 +826,52 @@
         <v/>
       </c>
       <c r="B4" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="8" t="n">
-        <v>71</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="K4" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="L4" s="24" t="n">
-        <v>0.7746478873239436</v>
-      </c>
-      <c r="M4" s="24" t="b">
+      <c r="L4" s="11" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="M4" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="N4" s="24" t="b">
+      <c r="N4" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="O4" s="24" t="b">
+      <c r="O4" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="P4" s="24" t="s">
-        <v>25</v>
+      <c r="P4" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -951,216 +879,88 @@
         <f>A4+1</f>
         <v/>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="15" t="n">
-        <v>70</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="26" t="n">
-        <v>0.6857142857142857</v>
-      </c>
-      <c r="M5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="B5" s="13" t="n"/>
+      <c r="C5" s="13" t="n"/>
+      <c r="D5" s="13" t="n"/>
+      <c r="E5" s="13" t="n"/>
+      <c r="F5" s="14" t="n"/>
+      <c r="G5" s="14" t="n"/>
+      <c r="H5" s="14" t="n"/>
+      <c r="I5" s="15" t="n"/>
+      <c r="J5" s="16" t="n"/>
+      <c r="K5" s="17" t="n"/>
+      <c r="L5" s="18" t="n"/>
+      <c r="M5" s="18" t="n"/>
+      <c r="N5" s="18" t="n"/>
+      <c r="O5" s="18" t="n"/>
+      <c r="P5" s="18" t="n"/>
+      <c r="Q5" s="19" t="n"/>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="5">
         <f>A5+1</f>
         <v/>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="8" t="n">
-        <v>135</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="24" t="n">
-        <v>0.7333333333333333</v>
-      </c>
-      <c r="M6" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="B6" s="6" t="n"/>
+      <c r="C6" s="6" t="n"/>
+      <c r="D6" s="6" t="n"/>
+      <c r="E6" s="6" t="n"/>
+      <c r="F6" s="9" t="n"/>
+      <c r="G6" s="9" t="n"/>
+      <c r="H6" s="9" t="n"/>
+      <c r="I6" s="8" t="n"/>
+      <c r="J6" s="20" t="n"/>
+      <c r="K6" s="10" t="n"/>
+      <c r="L6" s="11" t="n"/>
+      <c r="M6" s="11" t="n"/>
+      <c r="N6" s="11" t="n"/>
+      <c r="O6" s="11" t="n"/>
+      <c r="P6" s="11" t="n"/>
+      <c r="Q6" s="12" t="n"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="5">
         <f>A6+1</f>
         <v/>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="15" t="n">
-        <v>99</v>
-      </c>
-      <c r="J7" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="26" t="n">
-        <v>0.8080808080808081</v>
-      </c>
-      <c r="M7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="O7" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q7" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="B7" s="13" t="n"/>
+      <c r="C7" s="13" t="n"/>
+      <c r="D7" s="13" t="n"/>
+      <c r="E7" s="13" t="n"/>
+      <c r="F7" s="14" t="n"/>
+      <c r="G7" s="14" t="n"/>
+      <c r="H7" s="14" t="n"/>
+      <c r="I7" s="15" t="n"/>
+      <c r="J7" s="16" t="n"/>
+      <c r="K7" s="17" t="n"/>
+      <c r="L7" s="18" t="n"/>
+      <c r="M7" s="18" t="n"/>
+      <c r="N7" s="18" t="n"/>
+      <c r="O7" s="18" t="n"/>
+      <c r="P7" s="18" t="n"/>
+      <c r="Q7" s="19" t="n"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="5">
         <f>A7+1</f>
         <v/>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="8" t="n">
-        <v>140</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="K8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="24" t="n">
-        <v>0.5142857142857142</v>
-      </c>
-      <c r="M8" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="P8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="B8" s="6" t="n"/>
+      <c r="C8" s="6" t="n"/>
+      <c r="D8" s="6" t="n"/>
+      <c r="E8" s="6" t="n"/>
+      <c r="F8" s="9" t="n"/>
+      <c r="G8" s="9" t="n"/>
+      <c r="H8" s="9" t="n"/>
+      <c r="I8" s="8" t="n"/>
+      <c r="J8" s="20" t="n"/>
+      <c r="K8" s="10" t="n"/>
+      <c r="L8" s="11" t="n"/>
+      <c r="M8" s="11" t="n"/>
+      <c r="N8" s="11" t="n"/>
+      <c r="O8" s="11" t="n"/>
+      <c r="P8" s="11" t="n"/>
+      <c r="Q8" s="12" t="n"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="5">
@@ -1175,13 +975,13 @@
       <c r="G9" s="14" t="n"/>
       <c r="H9" s="14" t="n"/>
       <c r="I9" s="15" t="n"/>
-      <c r="J9" s="25" t="n"/>
+      <c r="J9" s="16" t="n"/>
       <c r="K9" s="17" t="n"/>
-      <c r="L9" s="26" t="n"/>
-      <c r="M9" s="26" t="n"/>
-      <c r="N9" s="26" t="n"/>
-      <c r="O9" s="26" t="n"/>
-      <c r="P9" s="26" t="n"/>
+      <c r="L9" s="18" t="n"/>
+      <c r="M9" s="18" t="n"/>
+      <c r="N9" s="18" t="n"/>
+      <c r="O9" s="18" t="n"/>
+      <c r="P9" s="18" t="n"/>
       <c r="Q9" s="19" t="n"/>
     </row>
     <row r="10" spans="1:17">
@@ -1197,13 +997,13 @@
       <c r="G10" s="9" t="n"/>
       <c r="H10" s="9" t="n"/>
       <c r="I10" s="8" t="n"/>
-      <c r="J10" s="27" t="n"/>
+      <c r="J10" s="20" t="n"/>
       <c r="K10" s="10" t="n"/>
-      <c r="L10" s="24" t="n"/>
-      <c r="M10" s="24" t="n"/>
-      <c r="N10" s="24" t="n"/>
-      <c r="O10" s="24" t="n"/>
-      <c r="P10" s="24" t="n"/>
+      <c r="L10" s="11" t="n"/>
+      <c r="M10" s="11" t="n"/>
+      <c r="N10" s="11" t="n"/>
+      <c r="O10" s="11" t="n"/>
+      <c r="P10" s="11" t="n"/>
       <c r="Q10" s="12" t="n"/>
     </row>
     <row r="11" spans="1:17">
@@ -1219,13 +1019,13 @@
       <c r="G11" s="14" t="n"/>
       <c r="H11" s="14" t="n"/>
       <c r="I11" s="15" t="n"/>
-      <c r="J11" s="25" t="n"/>
+      <c r="J11" s="16" t="n"/>
       <c r="K11" s="17" t="n"/>
-      <c r="L11" s="26" t="n"/>
-      <c r="M11" s="26" t="n"/>
-      <c r="N11" s="26" t="n"/>
-      <c r="O11" s="26" t="n"/>
-      <c r="P11" s="26" t="n"/>
+      <c r="L11" s="18" t="n"/>
+      <c r="M11" s="18" t="n"/>
+      <c r="N11" s="18" t="n"/>
+      <c r="O11" s="18" t="n"/>
+      <c r="P11" s="18" t="n"/>
       <c r="Q11" s="19" t="n"/>
     </row>
     <row r="12" spans="1:17">
@@ -1241,13 +1041,13 @@
       <c r="G12" s="9" t="n"/>
       <c r="H12" s="9" t="n"/>
       <c r="I12" s="8" t="n"/>
-      <c r="J12" s="27" t="n"/>
+      <c r="J12" s="20" t="n"/>
       <c r="K12" s="10" t="n"/>
-      <c r="L12" s="24" t="n"/>
-      <c r="M12" s="24" t="n"/>
-      <c r="N12" s="24" t="n"/>
-      <c r="O12" s="24" t="n"/>
-      <c r="P12" s="24" t="n"/>
+      <c r="L12" s="11" t="n"/>
+      <c r="M12" s="11" t="n"/>
+      <c r="N12" s="11" t="n"/>
+      <c r="O12" s="11" t="n"/>
+      <c r="P12" s="11" t="n"/>
       <c r="Q12" s="12" t="n"/>
     </row>
     <row r="13" spans="1:17">
@@ -1263,13 +1063,13 @@
       <c r="G13" s="14" t="n"/>
       <c r="H13" s="14" t="n"/>
       <c r="I13" s="15" t="n"/>
-      <c r="J13" s="25" t="n"/>
+      <c r="J13" s="16" t="n"/>
       <c r="K13" s="17" t="n"/>
-      <c r="L13" s="26" t="n"/>
-      <c r="M13" s="26" t="n"/>
-      <c r="N13" s="26" t="n"/>
-      <c r="O13" s="26" t="n"/>
-      <c r="P13" s="26" t="n"/>
+      <c r="L13" s="18" t="n"/>
+      <c r="M13" s="18" t="n"/>
+      <c r="N13" s="18" t="n"/>
+      <c r="O13" s="18" t="n"/>
+      <c r="P13" s="18" t="n"/>
       <c r="Q13" s="19" t="n"/>
     </row>
     <row r="14" spans="1:17">
@@ -1287,11 +1087,11 @@
       <c r="I14" s="8" t="n"/>
       <c r="J14" s="9" t="n"/>
       <c r="K14" s="10" t="n"/>
-      <c r="L14" s="24" t="n"/>
-      <c r="M14" s="24" t="n"/>
-      <c r="N14" s="24" t="n"/>
-      <c r="O14" s="24" t="n"/>
-      <c r="P14" s="24" t="n"/>
+      <c r="L14" s="11" t="n"/>
+      <c r="M14" s="11" t="n"/>
+      <c r="N14" s="11" t="n"/>
+      <c r="O14" s="11" t="n"/>
+      <c r="P14" s="11" t="n"/>
       <c r="Q14" s="12" t="n"/>
     </row>
     <row r="15" spans="1:17">
@@ -1307,13 +1107,13 @@
       <c r="G15" s="14" t="n"/>
       <c r="H15" s="14" t="n"/>
       <c r="I15" s="15" t="n"/>
-      <c r="J15" s="25" t="n"/>
+      <c r="J15" s="16" t="n"/>
       <c r="K15" s="17" t="n"/>
-      <c r="L15" s="26" t="n"/>
-      <c r="M15" s="26" t="n"/>
-      <c r="N15" s="26" t="n"/>
-      <c r="O15" s="26" t="n"/>
-      <c r="P15" s="26" t="n"/>
+      <c r="L15" s="18" t="n"/>
+      <c r="M15" s="18" t="n"/>
+      <c r="N15" s="18" t="n"/>
+      <c r="O15" s="18" t="n"/>
+      <c r="P15" s="18" t="n"/>
       <c r="Q15" s="19" t="n"/>
     </row>
     <row r="16" spans="1:17">
@@ -1331,11 +1131,11 @@
       <c r="I16" s="8" t="n"/>
       <c r="J16" s="9" t="n"/>
       <c r="K16" s="10" t="n"/>
-      <c r="L16" s="24" t="n"/>
-      <c r="M16" s="24" t="n"/>
-      <c r="N16" s="24" t="n"/>
-      <c r="O16" s="24" t="n"/>
-      <c r="P16" s="24" t="n"/>
+      <c r="L16" s="11" t="n"/>
+      <c r="M16" s="11" t="n"/>
+      <c r="N16" s="11" t="n"/>
+      <c r="O16" s="11" t="n"/>
+      <c r="P16" s="11" t="n"/>
       <c r="Q16" s="12" t="n"/>
     </row>
     <row r="17" spans="1:17">
@@ -1351,13 +1151,13 @@
       <c r="G17" s="14" t="n"/>
       <c r="H17" s="14" t="n"/>
       <c r="I17" s="15" t="n"/>
-      <c r="J17" s="25" t="n"/>
+      <c r="J17" s="16" t="n"/>
       <c r="K17" s="17" t="n"/>
-      <c r="L17" s="26" t="n"/>
-      <c r="M17" s="26" t="n"/>
-      <c r="N17" s="26" t="n"/>
-      <c r="O17" s="26" t="n"/>
-      <c r="P17" s="26" t="n"/>
+      <c r="L17" s="18" t="n"/>
+      <c r="M17" s="18" t="n"/>
+      <c r="N17" s="18" t="n"/>
+      <c r="O17" s="18" t="n"/>
+      <c r="P17" s="18" t="n"/>
       <c r="Q17" s="19" t="n"/>
     </row>
     <row r="18" spans="1:17">
@@ -1375,11 +1175,11 @@
       <c r="I18" s="8" t="n"/>
       <c r="J18" s="9" t="n"/>
       <c r="K18" s="10" t="n"/>
-      <c r="L18" s="24" t="n"/>
-      <c r="M18" s="24" t="n"/>
-      <c r="N18" s="24" t="n"/>
-      <c r="O18" s="24" t="n"/>
-      <c r="P18" s="24" t="n"/>
+      <c r="L18" s="11" t="n"/>
+      <c r="M18" s="11" t="n"/>
+      <c r="N18" s="11" t="n"/>
+      <c r="O18" s="11" t="n"/>
+      <c r="P18" s="11" t="n"/>
       <c r="Q18" s="12" t="n"/>
     </row>
     <row r="19" spans="1:17">
@@ -1395,13 +1195,13 @@
       <c r="G19" s="14" t="n"/>
       <c r="H19" s="14" t="n"/>
       <c r="I19" s="15" t="n"/>
-      <c r="J19" s="25" t="n"/>
+      <c r="J19" s="16" t="n"/>
       <c r="K19" s="17" t="n"/>
-      <c r="L19" s="26" t="n"/>
-      <c r="M19" s="26" t="n"/>
-      <c r="N19" s="26" t="n"/>
-      <c r="O19" s="26" t="n"/>
-      <c r="P19" s="26" t="n"/>
+      <c r="L19" s="18" t="n"/>
+      <c r="M19" s="18" t="n"/>
+      <c r="N19" s="18" t="n"/>
+      <c r="O19" s="18" t="n"/>
+      <c r="P19" s="18" t="n"/>
       <c r="Q19" s="19" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="20" spans="1:17">
@@ -1419,11 +1219,11 @@
       <c r="I20" s="8" t="n"/>
       <c r="J20" s="9" t="n"/>
       <c r="K20" s="10" t="n"/>
-      <c r="L20" s="24" t="n"/>
-      <c r="M20" s="24" t="n"/>
-      <c r="N20" s="24" t="n"/>
-      <c r="O20" s="24" t="n"/>
-      <c r="P20" s="24" t="n"/>
+      <c r="L20" s="11" t="n"/>
+      <c r="M20" s="11" t="n"/>
+      <c r="N20" s="11" t="n"/>
+      <c r="O20" s="11" t="n"/>
+      <c r="P20" s="11" t="n"/>
       <c r="Q20" s="12" t="n"/>
     </row>
     <row r="21" spans="1:17">
@@ -1439,13 +1239,13 @@
       <c r="G21" s="14" t="n"/>
       <c r="H21" s="14" t="n"/>
       <c r="I21" s="15" t="n"/>
-      <c r="J21" s="25" t="n"/>
+      <c r="J21" s="16" t="n"/>
       <c r="K21" s="17" t="n"/>
-      <c r="L21" s="26" t="n"/>
-      <c r="M21" s="26" t="n"/>
-      <c r="N21" s="26" t="n"/>
-      <c r="O21" s="26" t="n"/>
-      <c r="P21" s="26" t="n"/>
+      <c r="L21" s="18" t="n"/>
+      <c r="M21" s="18" t="n"/>
+      <c r="N21" s="18" t="n"/>
+      <c r="O21" s="18" t="n"/>
+      <c r="P21" s="18" t="n"/>
       <c r="Q21" s="19" t="n"/>
     </row>
     <row r="22" spans="1:17">
@@ -1463,11 +1263,11 @@
       <c r="I22" s="8" t="n"/>
       <c r="J22" s="9" t="n"/>
       <c r="K22" s="10" t="n"/>
-      <c r="L22" s="24" t="n"/>
-      <c r="M22" s="24" t="n"/>
-      <c r="N22" s="24" t="n"/>
-      <c r="O22" s="24" t="n"/>
-      <c r="P22" s="24" t="n"/>
+      <c r="L22" s="11" t="n"/>
+      <c r="M22" s="11" t="n"/>
+      <c r="N22" s="11" t="n"/>
+      <c r="O22" s="11" t="n"/>
+      <c r="P22" s="11" t="n"/>
       <c r="Q22" s="12" t="n"/>
     </row>
     <row r="23" spans="1:17">
@@ -1483,13 +1283,13 @@
       <c r="G23" s="14" t="n"/>
       <c r="H23" s="14" t="n"/>
       <c r="I23" s="15" t="n"/>
-      <c r="J23" s="25" t="n"/>
+      <c r="J23" s="16" t="n"/>
       <c r="K23" s="17" t="n"/>
-      <c r="L23" s="26" t="n"/>
-      <c r="M23" s="26" t="n"/>
-      <c r="N23" s="26" t="n"/>
-      <c r="O23" s="26" t="n"/>
-      <c r="P23" s="26" t="n"/>
+      <c r="L23" s="18" t="n"/>
+      <c r="M23" s="18" t="n"/>
+      <c r="N23" s="18" t="n"/>
+      <c r="O23" s="18" t="n"/>
+      <c r="P23" s="18" t="n"/>
       <c r="Q23" s="19" t="n"/>
     </row>
     <row r="24" spans="1:17">
@@ -1507,11 +1307,11 @@
       <c r="I24" s="8" t="n"/>
       <c r="J24" s="9" t="n"/>
       <c r="K24" s="10" t="n"/>
-      <c r="L24" s="24" t="n"/>
-      <c r="M24" s="24" t="n"/>
-      <c r="N24" s="24" t="n"/>
-      <c r="O24" s="24" t="n"/>
-      <c r="P24" s="24" t="n"/>
+      <c r="L24" s="11" t="n"/>
+      <c r="M24" s="11" t="n"/>
+      <c r="N24" s="11" t="n"/>
+      <c r="O24" s="11" t="n"/>
+      <c r="P24" s="11" t="n"/>
       <c r="Q24" s="12" t="n"/>
     </row>
     <row r="25" spans="1:17">
@@ -1527,13 +1327,13 @@
       <c r="G25" s="14" t="n"/>
       <c r="H25" s="14" t="n"/>
       <c r="I25" s="15" t="n"/>
-      <c r="J25" s="25" t="n"/>
+      <c r="J25" s="16" t="n"/>
       <c r="K25" s="17" t="n"/>
-      <c r="L25" s="26" t="n"/>
-      <c r="M25" s="26" t="n"/>
-      <c r="N25" s="26" t="n"/>
-      <c r="O25" s="26" t="n"/>
-      <c r="P25" s="26" t="n"/>
+      <c r="L25" s="18" t="n"/>
+      <c r="M25" s="18" t="n"/>
+      <c r="N25" s="18" t="n"/>
+      <c r="O25" s="18" t="n"/>
+      <c r="P25" s="18" t="n"/>
       <c r="Q25" s="19" t="n"/>
     </row>
     <row r="26" spans="1:17">
@@ -1551,11 +1351,11 @@
       <c r="I26" s="8" t="n"/>
       <c r="J26" s="9" t="n"/>
       <c r="K26" s="10" t="n"/>
-      <c r="L26" s="24" t="n"/>
-      <c r="M26" s="24" t="n"/>
-      <c r="N26" s="24" t="n"/>
-      <c r="O26" s="24" t="n"/>
-      <c r="P26" s="24" t="n"/>
+      <c r="L26" s="11" t="n"/>
+      <c r="M26" s="11" t="n"/>
+      <c r="N26" s="11" t="n"/>
+      <c r="O26" s="11" t="n"/>
+      <c r="P26" s="11" t="n"/>
       <c r="Q26" s="12" t="n"/>
     </row>
     <row r="27" spans="1:17">
@@ -1571,13 +1371,13 @@
       <c r="G27" s="14" t="n"/>
       <c r="H27" s="14" t="n"/>
       <c r="I27" s="15" t="n"/>
-      <c r="J27" s="25" t="n"/>
+      <c r="J27" s="16" t="n"/>
       <c r="K27" s="17" t="n"/>
-      <c r="L27" s="26" t="n"/>
-      <c r="M27" s="26" t="n"/>
-      <c r="N27" s="26" t="n"/>
-      <c r="O27" s="26" t="n"/>
-      <c r="P27" s="26" t="n"/>
+      <c r="L27" s="18" t="n"/>
+      <c r="M27" s="18" t="n"/>
+      <c r="N27" s="18" t="n"/>
+      <c r="O27" s="18" t="n"/>
+      <c r="P27" s="18" t="n"/>
       <c r="Q27" s="19" t="n"/>
     </row>
     <row r="28" spans="1:17">
@@ -1595,11 +1395,11 @@
       <c r="I28" s="8" t="n"/>
       <c r="J28" s="9" t="n"/>
       <c r="K28" s="10" t="n"/>
-      <c r="L28" s="24" t="n"/>
-      <c r="M28" s="24" t="n"/>
-      <c r="N28" s="24" t="n"/>
-      <c r="O28" s="24" t="n"/>
-      <c r="P28" s="24" t="n"/>
+      <c r="L28" s="11" t="n"/>
+      <c r="M28" s="11" t="n"/>
+      <c r="N28" s="11" t="n"/>
+      <c r="O28" s="11" t="n"/>
+      <c r="P28" s="11" t="n"/>
       <c r="Q28" s="12" t="n"/>
     </row>
     <row r="29" spans="1:17">
@@ -1615,13 +1415,13 @@
       <c r="G29" s="14" t="n"/>
       <c r="H29" s="14" t="n"/>
       <c r="I29" s="15" t="n"/>
-      <c r="J29" s="25" t="n"/>
+      <c r="J29" s="16" t="n"/>
       <c r="K29" s="17" t="n"/>
-      <c r="L29" s="26" t="n"/>
-      <c r="M29" s="26" t="n"/>
-      <c r="N29" s="26" t="n"/>
-      <c r="O29" s="26" t="n"/>
-      <c r="P29" s="26" t="n"/>
+      <c r="L29" s="18" t="n"/>
+      <c r="M29" s="18" t="n"/>
+      <c r="N29" s="18" t="n"/>
+      <c r="O29" s="18" t="n"/>
+      <c r="P29" s="18" t="n"/>
       <c r="Q29" s="19" t="n"/>
     </row>
     <row r="30" spans="1:17">
@@ -1639,11 +1439,11 @@
       <c r="I30" s="8" t="n"/>
       <c r="J30" s="9" t="n"/>
       <c r="K30" s="10" t="n"/>
-      <c r="L30" s="24" t="n"/>
-      <c r="M30" s="24" t="n"/>
-      <c r="N30" s="24" t="n"/>
-      <c r="O30" s="24" t="n"/>
-      <c r="P30" s="24" t="n"/>
+      <c r="L30" s="11" t="n"/>
+      <c r="M30" s="11" t="n"/>
+      <c r="N30" s="11" t="n"/>
+      <c r="O30" s="11" t="n"/>
+      <c r="P30" s="11" t="n"/>
       <c r="Q30" s="12" t="n"/>
     </row>
     <row r="31" spans="1:17">
@@ -1659,13 +1459,13 @@
       <c r="G31" s="14" t="n"/>
       <c r="H31" s="14" t="n"/>
       <c r="I31" s="15" t="n"/>
-      <c r="J31" s="25" t="n"/>
+      <c r="J31" s="16" t="n"/>
       <c r="K31" s="17" t="n"/>
-      <c r="L31" s="26" t="n"/>
-      <c r="M31" s="26" t="n"/>
-      <c r="N31" s="26" t="n"/>
-      <c r="O31" s="26" t="n"/>
-      <c r="P31" s="26" t="n"/>
+      <c r="L31" s="18" t="n"/>
+      <c r="M31" s="18" t="n"/>
+      <c r="N31" s="18" t="n"/>
+      <c r="O31" s="18" t="n"/>
+      <c r="P31" s="18" t="n"/>
       <c r="Q31" s="19" t="n"/>
     </row>
     <row r="32" spans="1:17">
@@ -1683,11 +1483,11 @@
       <c r="I32" s="8" t="n"/>
       <c r="J32" s="9" t="n"/>
       <c r="K32" s="10" t="n"/>
-      <c r="L32" s="24" t="n"/>
-      <c r="M32" s="24" t="n"/>
-      <c r="N32" s="24" t="n"/>
-      <c r="O32" s="24" t="n"/>
-      <c r="P32" s="24" t="n"/>
+      <c r="L32" s="11" t="n"/>
+      <c r="M32" s="11" t="n"/>
+      <c r="N32" s="11" t="n"/>
+      <c r="O32" s="11" t="n"/>
+      <c r="P32" s="11" t="n"/>
       <c r="Q32" s="12" t="n"/>
     </row>
     <row r="33" spans="1:17">
@@ -1703,13 +1503,13 @@
       <c r="G33" s="14" t="n"/>
       <c r="H33" s="14" t="n"/>
       <c r="I33" s="15" t="n"/>
-      <c r="J33" s="25" t="n"/>
+      <c r="J33" s="16" t="n"/>
       <c r="K33" s="17" t="n"/>
-      <c r="L33" s="26" t="n"/>
-      <c r="M33" s="26" t="n"/>
-      <c r="N33" s="26" t="n"/>
-      <c r="O33" s="26" t="n"/>
-      <c r="P33" s="26" t="n"/>
+      <c r="L33" s="18" t="n"/>
+      <c r="M33" s="18" t="n"/>
+      <c r="N33" s="18" t="n"/>
+      <c r="O33" s="18" t="n"/>
+      <c r="P33" s="18" t="n"/>
       <c r="Q33" s="19" t="n"/>
     </row>
     <row r="34" spans="1:17">
@@ -1727,11 +1527,11 @@
       <c r="I34" s="8" t="n"/>
       <c r="J34" s="9" t="n"/>
       <c r="K34" s="10" t="n"/>
-      <c r="L34" s="24" t="n"/>
-      <c r="M34" s="24" t="n"/>
-      <c r="N34" s="24" t="n"/>
-      <c r="O34" s="24" t="n"/>
-      <c r="P34" s="24" t="n"/>
+      <c r="L34" s="11" t="n"/>
+      <c r="M34" s="11" t="n"/>
+      <c r="N34" s="11" t="n"/>
+      <c r="O34" s="11" t="n"/>
+      <c r="P34" s="11" t="n"/>
       <c r="Q34" s="12" t="n"/>
     </row>
     <row r="35" spans="1:17">
@@ -1747,13 +1547,13 @@
       <c r="G35" s="14" t="n"/>
       <c r="H35" s="14" t="n"/>
       <c r="I35" s="15" t="n"/>
-      <c r="J35" s="25" t="n"/>
+      <c r="J35" s="16" t="n"/>
       <c r="K35" s="17" t="n"/>
-      <c r="L35" s="26" t="n"/>
-      <c r="M35" s="26" t="n"/>
-      <c r="N35" s="26" t="n"/>
-      <c r="O35" s="26" t="n"/>
-      <c r="P35" s="26" t="n"/>
+      <c r="L35" s="18" t="n"/>
+      <c r="M35" s="18" t="n"/>
+      <c r="N35" s="18" t="n"/>
+      <c r="O35" s="18" t="n"/>
+      <c r="P35" s="18" t="n"/>
       <c r="Q35" s="19" t="n"/>
     </row>
     <row r="36" spans="1:17">
@@ -1771,11 +1571,11 @@
       <c r="I36" s="8" t="n"/>
       <c r="J36" s="9" t="n"/>
       <c r="K36" s="10" t="n"/>
-      <c r="L36" s="24" t="n"/>
-      <c r="M36" s="24" t="n"/>
-      <c r="N36" s="24" t="n"/>
-      <c r="O36" s="24" t="n"/>
-      <c r="P36" s="24" t="n"/>
+      <c r="L36" s="11" t="n"/>
+      <c r="M36" s="11" t="n"/>
+      <c r="N36" s="11" t="n"/>
+      <c r="O36" s="11" t="n"/>
+      <c r="P36" s="11" t="n"/>
       <c r="Q36" s="12" t="n"/>
     </row>
     <row r="37" spans="1:17">
@@ -1791,13 +1591,13 @@
       <c r="G37" s="14" t="n"/>
       <c r="H37" s="14" t="n"/>
       <c r="I37" s="15" t="n"/>
-      <c r="J37" s="25" t="n"/>
+      <c r="J37" s="16" t="n"/>
       <c r="K37" s="17" t="n"/>
-      <c r="L37" s="26" t="n"/>
-      <c r="M37" s="26" t="n"/>
-      <c r="N37" s="26" t="n"/>
-      <c r="O37" s="26" t="n"/>
-      <c r="P37" s="26" t="n"/>
+      <c r="L37" s="18" t="n"/>
+      <c r="M37" s="18" t="n"/>
+      <c r="N37" s="18" t="n"/>
+      <c r="O37" s="18" t="n"/>
+      <c r="P37" s="18" t="n"/>
       <c r="Q37" s="19" t="n"/>
     </row>
     <row r="38" spans="1:17">
@@ -1815,11 +1615,11 @@
       <c r="I38" s="8" t="n"/>
       <c r="J38" s="9" t="n"/>
       <c r="K38" s="10" t="n"/>
-      <c r="L38" s="24" t="n"/>
-      <c r="M38" s="24" t="n"/>
-      <c r="N38" s="24" t="n"/>
-      <c r="O38" s="24" t="n"/>
-      <c r="P38" s="24" t="n"/>
+      <c r="L38" s="11" t="n"/>
+      <c r="M38" s="11" t="n"/>
+      <c r="N38" s="11" t="n"/>
+      <c r="O38" s="11" t="n"/>
+      <c r="P38" s="11" t="n"/>
       <c r="Q38" s="12" t="n"/>
     </row>
     <row r="39" spans="1:17">
@@ -1835,13 +1635,13 @@
       <c r="G39" s="14" t="n"/>
       <c r="H39" s="14" t="n"/>
       <c r="I39" s="15" t="n"/>
-      <c r="J39" s="25" t="n"/>
+      <c r="J39" s="16" t="n"/>
       <c r="K39" s="17" t="n"/>
-      <c r="L39" s="26" t="n"/>
-      <c r="M39" s="26" t="n"/>
-      <c r="N39" s="26" t="n"/>
-      <c r="O39" s="26" t="n"/>
-      <c r="P39" s="26" t="n"/>
+      <c r="L39" s="18" t="n"/>
+      <c r="M39" s="18" t="n"/>
+      <c r="N39" s="18" t="n"/>
+      <c r="O39" s="18" t="n"/>
+      <c r="P39" s="18" t="n"/>
       <c r="Q39" s="19" t="n"/>
     </row>
     <row r="40" spans="1:17">
@@ -1859,11 +1659,11 @@
       <c r="I40" s="8" t="n"/>
       <c r="J40" s="9" t="n"/>
       <c r="K40" s="10" t="n"/>
-      <c r="L40" s="24" t="n"/>
-      <c r="M40" s="24" t="n"/>
-      <c r="N40" s="24" t="n"/>
-      <c r="O40" s="24" t="n"/>
-      <c r="P40" s="24" t="n"/>
+      <c r="L40" s="11" t="n"/>
+      <c r="M40" s="11" t="n"/>
+      <c r="N40" s="11" t="n"/>
+      <c r="O40" s="11" t="n"/>
+      <c r="P40" s="11" t="n"/>
       <c r="Q40" s="12" t="n"/>
     </row>
     <row r="41" spans="1:17">
@@ -1879,13 +1679,13 @@
       <c r="G41" s="14" t="n"/>
       <c r="H41" s="14" t="n"/>
       <c r="I41" s="15" t="n"/>
-      <c r="J41" s="25" t="n"/>
+      <c r="J41" s="16" t="n"/>
       <c r="K41" s="17" t="n"/>
-      <c r="L41" s="26" t="n"/>
-      <c r="M41" s="26" t="n"/>
-      <c r="N41" s="26" t="n"/>
-      <c r="O41" s="26" t="n"/>
-      <c r="P41" s="26" t="n"/>
+      <c r="L41" s="18" t="n"/>
+      <c r="M41" s="18" t="n"/>
+      <c r="N41" s="18" t="n"/>
+      <c r="O41" s="18" t="n"/>
+      <c r="P41" s="18" t="n"/>
       <c r="Q41" s="19" t="n"/>
     </row>
     <row r="42" spans="1:17">
@@ -1903,11 +1703,11 @@
       <c r="I42" s="8" t="n"/>
       <c r="J42" s="9" t="n"/>
       <c r="K42" s="10" t="n"/>
-      <c r="L42" s="24" t="n"/>
-      <c r="M42" s="24" t="n"/>
-      <c r="N42" s="24" t="n"/>
-      <c r="O42" s="24" t="n"/>
-      <c r="P42" s="24" t="n"/>
+      <c r="L42" s="11" t="n"/>
+      <c r="M42" s="11" t="n"/>
+      <c r="N42" s="11" t="n"/>
+      <c r="O42" s="11" t="n"/>
+      <c r="P42" s="11" t="n"/>
       <c r="Q42" s="12" t="n"/>
     </row>
     <row r="43" spans="1:17">
@@ -1927,15 +1727,15 @@
       </c>
       <c r="J43" s="3" t="n"/>
       <c r="K43" s="3" t="n"/>
-      <c r="L43" s="28">
+      <c r="L43" s="22">
         <f>AVERAGE(L3:L42)</f>
         <v/>
       </c>
-      <c r="M43" s="28" t="n"/>
-      <c r="N43" s="28" t="n"/>
-      <c r="O43" s="28" t="n"/>
-      <c r="P43" s="28" t="n"/>
-      <c r="Q43" s="29">
+      <c r="M43" s="22" t="n"/>
+      <c r="N43" s="22" t="n"/>
+      <c r="O43" s="22" t="n"/>
+      <c r="P43" s="22" t="n"/>
+      <c r="Q43" s="23">
         <f>AVERAGE(Q2:Q42)</f>
         <v/>
       </c>

</xml_diff>